<commit_message>
Changes to BowelFunction mapping as we try to get a unified way to write down the use of extensions
</commit_message>
<xml_diff>
--- a/Mappings/BowelFunction - STU3.xlsx
+++ b/Mappings/BowelFunction - STU3.xlsx
@@ -1,16 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Edelman\Nictiz-STU3-Zib2017\Mappings\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{135853BC-4B8C-48EA-B005-E27D62C04244}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="630" yWindow="615" windowWidth="27495" windowHeight="11955" firstSheet="3" activeTab="4"/>
+    <workbookView xWindow="630" yWindow="615" windowWidth="27495" windowHeight="11955" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="Metadata" sheetId="2" r:id="rId2"/>
     <sheet name="Information Model" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet1" sheetId="9" r:id="rId4"/>
+    <sheet name="Research" sheetId="9" r:id="rId4"/>
     <sheet name="Data" sheetId="4" r:id="rId5"/>
     <sheet name="DefecationColorCodelist" sheetId="5" r:id="rId6"/>
     <sheet name="DefecationConsistencyCodelist" sheetId="6" r:id="rId7"/>
@@ -18,19 +24,11 @@
     <sheet name="Terms of Use" sheetId="8" r:id="rId9"/>
   </sheets>
   <calcPr calcId="145621"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="221">
   <si>
     <t>Subject</t>
   </si>
@@ -312,9 +310,6 @@
     <t>This is a reference to the rootconcept of information model Stoma.</t>
   </si>
   <si>
-    <t>.stoma (extension, reference to HCIM Stoma</t>
-  </si>
-  <si>
     <t>Frequency</t>
   </si>
   <si>
@@ -333,9 +328,6 @@
     <t>SNOMED CT: 162098000 Frequency of defecation</t>
   </si>
   <si>
-    <t>.Component.frequency.valueString</t>
-  </si>
-  <si>
     <t>DefecationConsistency</t>
   </si>
   <si>
@@ -357,9 +349,6 @@
     <t>DefecationConsistencyCodelist</t>
   </si>
   <si>
-    <t>.component.defecationConsistency.valueCodeableConcept</t>
-  </si>
-  <si>
     <t>DefecationColor</t>
   </si>
   <si>
@@ -399,9 +388,6 @@
     <t>This is a reference to the rootconcept of information model MedicalDevice.</t>
   </si>
   <si>
-    <t>.incontinence (extension, reference to MedicalDevice)</t>
-  </si>
-  <si>
     <t>Comment</t>
   </si>
   <si>
@@ -694,13 +680,29 @@
   </si>
   <si>
     <t>Valueset reference</t>
+  </si>
+  <si>
+    <t>.component.frequency.valueQuantity</t>
+  </si>
+  <si>
+    <t>.component.defecationConsistency.valueCodeableconcept</t>
+  </si>
+  <si>
+    <t>.incontinenceMaterial.valueReference.device.type, where:
+- .incontinenceMaterial (extension http://nictiz.nl/fhir/StructureDefinition/extension-medicaldevice)
+- .incontinenceMaterial.valueReference (profile http://nictiz.nl/fhir/StructureDefinition/zib-MedicalDevice)
+- .incontinenceMaterial.valueReference.device (profile http://nictiz.nl/fhir/StructureDefinition/zib-MedicalDeviceProduct)</t>
+  </si>
+  <si>
+    <t>.stoma.valueReference, where
+- .stoma (extension zib-BowelFunction-Stoma, reference to HCIM Stoma)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Calibri"/>
@@ -710,23 +712,27 @@
       <sz val="10"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -827,7 +833,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -874,9 +880,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
@@ -884,9 +887,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1036,7 +1049,7 @@
         <xdr:cNvPr id="1025" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000001040000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1077,7 +1090,7 @@
         <xdr:cNvPr id="1026" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002040000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1118,7 +1131,7 @@
         <xdr:cNvPr id="1025" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000001040000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000001040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1173,11 +1186,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3073"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000010C0000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1185,6 +1201,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1214,11 +1253,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3074"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000020C0000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1226,6 +1268,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1255,11 +1320,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3075"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000030C0000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1267,6 +1335,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1296,11 +1387,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3076"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000040C0000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1308,6 +1402,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1337,11 +1454,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3077"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000050C0000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1349,6 +1469,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1378,11 +1521,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3078"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000060C0000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1390,6 +1536,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1419,11 +1588,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3079"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000070C0000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1431,6 +1603,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1460,11 +1655,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3080"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000080C0000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1472,6 +1670,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1501,11 +1722,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3081"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000090C0000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1513,6 +1737,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1542,11 +1789,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3082"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000A0C0000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1554,6 +1804,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1583,11 +1856,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3083"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000B0C0000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1595,6 +1871,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1624,11 +1923,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3084"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000C0C0000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1636,6 +1938,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1665,11 +1990,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3085"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000D0C0000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1677,6 +2005,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1706,11 +2057,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3086"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000E0C0000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1718,6 +2072,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1747,11 +2124,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3087"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000F0C0000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1759,6 +2139,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1788,11 +2191,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3088"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000100C0000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1800,6 +2206,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1829,11 +2258,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3089"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000110C0000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1841,6 +2273,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1870,11 +2325,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3090"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000120C0000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1882,6 +2340,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1911,11 +2392,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3091"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000130C0000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1923,6 +2407,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1952,11 +2459,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3092"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000140C0000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1964,6 +2474,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1993,11 +2526,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3093"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000150C0000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2005,6 +2541,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2034,11 +2593,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3094"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000160C0000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2046,6 +2608,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2075,11 +2660,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3095"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000170C0000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2087,6 +2675,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2116,11 +2727,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3096"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000180C0000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2128,6 +2742,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2157,11 +2794,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3097"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000190C0000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2169,6 +2809,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2198,11 +2861,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3098"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00001A0C0000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2210,6 +2876,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2239,11 +2928,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3099"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00001B0C0000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2251,6 +2943,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2280,11 +2995,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3100"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00001C0C0000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2292,6 +3010,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2321,11 +3062,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3101"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00001D0C0000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2333,6 +3077,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2362,11 +3129,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3102"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00001E0C0000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2374,6 +3144,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2385,7 +3178,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2427,7 +3220,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2460,9 +3253,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2495,6 +3305,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2670,18 +3497,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="15" customWidth="1"/>
     <col min="3" max="3" width="100" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B2" s="14" t="s">
         <v>0</v>
       </c>
@@ -2689,7 +3516,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:3">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
@@ -2697,7 +3524,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:3">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
@@ -2705,7 +3532,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="2:3">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
@@ -2713,7 +3540,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="2:3">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
         <v>8</v>
       </c>
@@ -2721,7 +3548,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="2:3">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
         <v>10</v>
       </c>
@@ -2729,7 +3556,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="2:3">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
         <v>12</v>
       </c>
@@ -2737,7 +3564,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="2:3">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
         <v>14</v>
       </c>
@@ -2745,7 +3572,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="2:3">
+    <row r="10" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
         <v>16</v>
       </c>
@@ -2753,7 +3580,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="2:3">
+    <row r="11" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
         <v>18</v>
       </c>
@@ -2761,7 +3588,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="2:3" ht="25.5">
+    <row r="12" spans="2:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
         <v>20</v>
       </c>
@@ -2769,7 +3596,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="2:3" ht="51">
+    <row r="13" spans="2:3" ht="51" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
         <v>22</v>
       </c>
@@ -2777,7 +3604,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="2:3">
+    <row r="14" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
         <v>24</v>
       </c>
@@ -2787,7 +3614,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C11" r:id="rId1"/>
+    <hyperlink ref="C11" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
@@ -2798,24 +3625,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:C25"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="35" customWidth="1"/>
     <col min="3" max="3" width="70" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3">
-      <c r="B2" s="16" t="s">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B2" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="16"/>
-    </row>
-    <row r="3" spans="2:3">
+      <c r="C2" s="21"/>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
         <v>27</v>
       </c>
@@ -2823,7 +3650,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="2:3">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
         <v>29</v>
       </c>
@@ -2831,7 +3658,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="2:3">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B5" s="1" t="s">
         <v>31</v>
       </c>
@@ -2839,7 +3666,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="2:3">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
         <v>32</v>
       </c>
@@ -2847,7 +3674,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="2:3">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
         <v>33</v>
       </c>
@@ -2855,7 +3682,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="2:3">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
         <v>34</v>
       </c>
@@ -2863,13 +3690,13 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="2:3">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
         <v>36</v>
       </c>
       <c r="C9" s="1"/>
     </row>
-    <row r="10" spans="2:3">
+    <row r="10" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
         <v>37</v>
       </c>
@@ -2877,13 +3704,13 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="2:3">
+    <row r="11" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C11" s="1"/>
     </row>
-    <row r="12" spans="2:3">
+    <row r="12" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
         <v>40</v>
       </c>
@@ -2891,13 +3718,13 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="2:3">
+    <row r="13" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
         <v>42</v>
       </c>
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="2:3">
+    <row r="14" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
         <v>43</v>
       </c>
@@ -2905,7 +3732,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="2:3">
+    <row r="15" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
         <v>45</v>
       </c>
@@ -2913,7 +3740,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="16" spans="2:3">
+    <row r="16" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
         <v>47</v>
       </c>
@@ -2921,7 +3748,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="2:3">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
         <v>48</v>
       </c>
@@ -2929,7 +3756,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="2:3">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
         <v>49</v>
       </c>
@@ -2937,7 +3764,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="2:3">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
         <v>51</v>
       </c>
@@ -2945,7 +3772,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="2:3">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
         <v>52</v>
       </c>
@@ -2953,7 +3780,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="2:3">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
         <v>53</v>
       </c>
@@ -2961,7 +3788,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="22" spans="2:3">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
         <v>55</v>
       </c>
@@ -2969,7 +3796,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="2:3">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
         <v>56</v>
       </c>
@@ -2977,7 +3804,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="24" spans="2:3">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
         <v>58</v>
       </c>
@@ -2985,7 +3812,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="2:3">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B25" s="1" t="s">
         <v>59</v>
       </c>
@@ -3005,14 +3832,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
     </row>
   </sheetData>
@@ -3022,106 +3849,106 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:O10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="46.5703125" customWidth="1"/>
     <col min="3" max="3" width="27.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="42" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A1" s="16" t="s">
+        <v>195</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>196</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>197</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>198</v>
+      </c>
+      <c r="E1" s="16" t="s">
         <v>199</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="O1" s="16"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A2" s="17" t="s">
         <v>200</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C2" s="17" t="s">
+        <v>210</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>208</v>
+      </c>
+      <c r="E2" s="17"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A3" s="17" t="s">
         <v>201</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D3" s="17"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A4" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="D4" s="17"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A5" s="17" t="s">
         <v>203</v>
       </c>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="O1" s="17"/>
-    </row>
-    <row r="2" spans="1:15">
-      <c r="A2" s="18" t="s">
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A6" s="17" t="s">
         <v>204</v>
       </c>
-      <c r="C2" s="18" t="s">
-        <v>214</v>
-      </c>
-      <c r="D2" s="19" t="s">
-        <v>212</v>
-      </c>
-      <c r="E2" s="18"/>
-    </row>
-    <row r="3" spans="1:15">
-      <c r="A3" s="18" t="s">
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A7" s="17" t="s">
         <v>205</v>
       </c>
-      <c r="D3" s="18"/>
-    </row>
-    <row r="4" spans="1:15">
-      <c r="A4" s="18" t="s">
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A8" s="17" t="s">
         <v>206</v>
       </c>
-      <c r="D4" s="18"/>
-    </row>
-    <row r="5" spans="1:15">
-      <c r="A5" s="18" t="s">
+      <c r="C8" s="17" t="s">
+        <v>210</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>208</v>
+      </c>
+      <c r="E8" s="17"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A9" s="17" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="6" spans="1:15">
-      <c r="A6" s="18" t="s">
+      <c r="C9" s="17" t="s">
+        <v>210</v>
+      </c>
+      <c r="D9" s="18" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
-      <c r="A7" s="18" t="s">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A10" s="17" t="s">
         <v>209</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15">
-      <c r="A8" s="18" t="s">
-        <v>210</v>
-      </c>
-      <c r="C8" s="18" t="s">
-        <v>214</v>
-      </c>
-      <c r="D8" s="19" t="s">
-        <v>212</v>
-      </c>
-      <c r="E8" s="18"/>
-    </row>
-    <row r="9" spans="1:15">
-      <c r="A9" s="18" t="s">
-        <v>211</v>
-      </c>
-      <c r="C9" s="18" t="s">
-        <v>214</v>
-      </c>
-      <c r="D9" s="19" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15">
-      <c r="A10" s="18" t="s">
-        <v>213</v>
       </c>
     </row>
   </sheetData>
@@ -3798,14 +4625,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="B2:T10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
       <selection activeCell="P6" sqref="P6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="6" width="2" customWidth="1"/>
     <col min="7" max="7" width="15" customWidth="1"/>
@@ -3816,12 +4643,14 @@
     <col min="13" max="13" width="75" customWidth="1"/>
     <col min="14" max="14" width="20" customWidth="1"/>
     <col min="15" max="15" width="30" customWidth="1"/>
-    <col min="16" max="18" width="46.28515625" customWidth="1"/>
+    <col min="16" max="16" width="93.28515625" customWidth="1"/>
+    <col min="17" max="17" width="11.7109375" customWidth="1"/>
+    <col min="18" max="18" width="8" customWidth="1"/>
     <col min="19" max="19" width="30" customWidth="1"/>
     <col min="20" max="20" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:20">
+    <row r="2" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B2" s="4" t="s">
         <v>20</v>
       </c>
@@ -3855,22 +4684,22 @@
         <v>68</v>
       </c>
       <c r="P2" s="14" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="Q2" s="15" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="R2" s="15" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="S2" s="14" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="T2" s="14" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="2:20" ht="25.5">
+    <row r="3" spans="2:20" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B3" s="7" t="s">
         <v>70</v>
       </c>
@@ -3903,11 +4732,11 @@
       <c r="Q3" s="3"/>
       <c r="R3" s="3"/>
       <c r="S3" s="3" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="T3" s="3"/>
     </row>
-    <row r="4" spans="2:20" ht="38.25">
+    <row r="4" spans="2:20" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B4" s="10"/>
       <c r="C4" s="11" t="s">
         <v>77</v>
@@ -3940,17 +4769,17 @@
       <c r="O4" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="P4" s="20" t="s">
+      <c r="P4" s="19" t="s">
         <v>86</v>
       </c>
-      <c r="Q4" s="20"/>
-      <c r="R4" s="20" t="s">
+      <c r="Q4" s="19"/>
+      <c r="R4" s="19" t="s">
         <v>2</v>
       </c>
       <c r="S4" s="2"/>
       <c r="T4" s="1"/>
     </row>
-    <row r="5" spans="2:20" ht="38.25">
+    <row r="5" spans="2:20" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B5" s="10"/>
       <c r="C5" s="11" t="s">
         <v>87</v>
@@ -3979,28 +4808,28 @@
       <c r="O5" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="P5" s="20" t="s">
-        <v>93</v>
-      </c>
-      <c r="Q5" s="20"/>
-      <c r="R5" s="20"/>
+      <c r="P5" s="24" t="s">
+        <v>220</v>
+      </c>
+      <c r="Q5" s="19"/>
+      <c r="R5" s="19"/>
       <c r="S5" s="2"/>
       <c r="T5" s="1"/>
     </row>
-    <row r="6" spans="2:20" ht="38.25">
+    <row r="6" spans="2:20" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B6" s="10"/>
       <c r="C6" s="11" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
       <c r="F6" s="11"/>
       <c r="G6" s="12"/>
       <c r="H6" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="I6" s="1" t="s">
         <v>95</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>96</v>
       </c>
       <c r="J6" s="1" t="s">
         <v>80</v>
@@ -4009,37 +4838,37 @@
         <v>81</v>
       </c>
       <c r="L6" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="M6" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="M6" s="1" t="s">
+      <c r="N6" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="N6" s="1" t="s">
-        <v>99</v>
-      </c>
       <c r="O6" s="1"/>
-      <c r="P6" s="20" t="s">
-        <v>100</v>
-      </c>
-      <c r="Q6" s="20"/>
-      <c r="R6" s="20"/>
+      <c r="P6" s="22" t="s">
+        <v>217</v>
+      </c>
+      <c r="Q6" s="19"/>
+      <c r="R6" s="19"/>
       <c r="S6" s="1"/>
       <c r="T6" s="1"/>
     </row>
-    <row r="7" spans="2:20" ht="38.25">
+    <row r="7" spans="2:20" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B7" s="10"/>
       <c r="C7" s="11" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
       <c r="F7" s="11"/>
       <c r="G7" s="12"/>
       <c r="H7" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="J7" s="1" t="s">
         <v>80</v>
@@ -4048,41 +4877,41 @@
         <v>81</v>
       </c>
       <c r="L7" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="N7" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="M7" s="1" t="s">
+      <c r="O7" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="N7" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="O7" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="P7" s="21" t="s">
-        <v>108</v>
-      </c>
-      <c r="Q7" s="21"/>
-      <c r="R7" s="21" t="s">
+      <c r="P7" s="23" t="s">
+        <v>218</v>
+      </c>
+      <c r="Q7" s="20"/>
+      <c r="R7" s="20" t="s">
         <v>2</v>
       </c>
       <c r="S7" s="2"/>
       <c r="T7" s="1"/>
     </row>
-    <row r="8" spans="2:20" ht="25.5">
+    <row r="8" spans="2:20" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B8" s="10"/>
       <c r="C8" s="11" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
       <c r="F8" s="11"/>
       <c r="G8" s="12"/>
       <c r="H8" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="J8" s="1" t="s">
         <v>80</v>
@@ -4091,36 +4920,38 @@
         <v>81</v>
       </c>
       <c r="L8" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="O8" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="M8" s="1" t="s">
+      <c r="P8" s="23" t="s">
         <v>112</v>
       </c>
-      <c r="N8" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="O8" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="P8" s="21" t="s">
-        <v>115</v>
-      </c>
-      <c r="Q8" s="21"/>
-      <c r="R8" s="21"/>
+      <c r="Q8" s="20"/>
+      <c r="R8" s="20" t="s">
+        <v>2</v>
+      </c>
       <c r="S8" s="2"/>
       <c r="T8" s="1"/>
     </row>
-    <row r="9" spans="2:20" ht="38.25">
+    <row r="9" spans="2:20" ht="63.75" x14ac:dyDescent="0.2">
       <c r="B9" s="10"/>
       <c r="C9" s="11" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
       <c r="F9" s="11"/>
       <c r="G9" s="12"/>
       <c r="H9" s="1" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="1" t="s">
@@ -4130,39 +4961,39 @@
         <v>89</v>
       </c>
       <c r="L9" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="O9" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="M9" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="N9" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="O9" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="P9" s="21" t="s">
-        <v>122</v>
-      </c>
-      <c r="Q9" s="21"/>
-      <c r="R9" s="21"/>
+      <c r="P9" s="23" t="s">
+        <v>219</v>
+      </c>
+      <c r="Q9" s="20"/>
+      <c r="R9" s="20"/>
       <c r="S9" s="2"/>
       <c r="T9" s="1"/>
     </row>
-    <row r="10" spans="2:20" ht="25.5">
+    <row r="10" spans="2:20" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B10" s="10"/>
       <c r="C10" s="11" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D10" s="11"/>
       <c r="E10" s="11"/>
       <c r="F10" s="11"/>
       <c r="G10" s="12"/>
       <c r="H10" s="1" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="J10" s="1" t="s">
         <v>80</v>
@@ -4171,34 +5002,35 @@
         <v>81</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="O10" s="1"/>
-      <c r="P10" s="21" t="s">
-        <v>129</v>
-      </c>
-      <c r="Q10" s="21" t="s">
-        <v>219</v>
-      </c>
-      <c r="R10" s="21"/>
+      <c r="P10" s="20" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q10" s="20" t="s">
+        <v>215</v>
+      </c>
+      <c r="R10" s="20"/>
       <c r="S10" s="1"/>
       <c r="T10" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="O4" location="FecalContinenceCodelist!A1" display="FecalContinenceCodelist"/>
-    <hyperlink ref="O5" r:id="rId1"/>
-    <hyperlink ref="O7" location="DefecationConsistencyCodelist!A1" display="DefecationConsistencyCodelist"/>
-    <hyperlink ref="O8" location="DefecationColorCodelist!A1" display="DefecationColorCodelist"/>
-    <hyperlink ref="O9" r:id="rId2"/>
+    <hyperlink ref="O4" location="FecalContinenceCodelist!A1" display="FecalContinenceCodelist" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
+    <hyperlink ref="O5" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
+    <hyperlink ref="O7" location="DefecationConsistencyCodelist!A1" display="DefecationConsistencyCodelist" xr:uid="{00000000-0004-0000-0400-000002000000}"/>
+    <hyperlink ref="O8" location="DefecationColorCodelist!A1" display="DefecationColorCodelist" xr:uid="{00000000-0004-0000-0400-000003000000}"/>
+    <hyperlink ref="O9" r:id="rId2" xr:uid="{00000000-0004-0000-0400-000004000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
   <ignoredErrors>
     <ignoredError sqref="J3:J9" numberStoredAsText="1"/>
   </ignoredErrors>
@@ -4206,12 +5038,12 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="C3:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="24" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
@@ -4220,134 +5052,134 @@
     <col min="7" max="7" width="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:7">
-      <c r="C3" s="16" t="s">
-        <v>114</v>
-      </c>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16" t="s">
+    <row r="3" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C3" s="21" t="s">
+        <v>111</v>
+      </c>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+    </row>
+    <row r="4" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C4" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="F4" s="13" t="s">
         <v>130</v>
-      </c>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
-    </row>
-    <row r="4" spans="3:7">
-      <c r="C4" s="13" t="s">
-        <v>131</v>
-      </c>
-      <c r="D4" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="E4" s="13" t="s">
-        <v>133</v>
-      </c>
-      <c r="F4" s="13" t="s">
-        <v>134</v>
       </c>
       <c r="G4" s="13" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="3:7">
+    <row r="5" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C5" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="D5" s="1" t="s">
+    </row>
+    <row r="6" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C6" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="E6" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="G5" s="1" t="s">
+    </row>
+    <row r="7" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C7" s="1" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="6" spans="3:7">
-      <c r="C6" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="E7" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="G7" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="G6" s="1" t="s">
+    </row>
+    <row r="8" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C8" s="1" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="7" spans="3:7">
-      <c r="C7" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="E8" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="G8" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="G7" s="1" t="s">
+    </row>
+    <row r="9" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C9" s="1" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="8" spans="3:7">
-      <c r="C8" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="E9" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="G8" s="1" t="s">
+    </row>
+    <row r="10" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C10" s="1" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="9" spans="3:7">
-      <c r="C9" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="E10" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="G10" s="1" t="s">
         <v>150</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="10" spans="3:7">
-      <c r="C10" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>154</v>
       </c>
     </row>
   </sheetData>
@@ -4363,12 +5195,12 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="C3:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="24" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
@@ -4377,151 +5209,151 @@
     <col min="7" max="7" width="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:7">
-      <c r="C3" s="16" t="s">
-        <v>107</v>
-      </c>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16" t="s">
-        <v>155</v>
-      </c>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
-    </row>
-    <row r="4" spans="3:7">
+    <row r="3" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C3" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21" t="s">
+        <v>151</v>
+      </c>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+    </row>
+    <row r="4" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C4" s="13" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="F4" s="13" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="G4" s="13" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="3:7" ht="25.5">
+    <row r="5" spans="3:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="C5" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="D5" s="1" t="s">
+    </row>
+    <row r="6" spans="3:7" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="C6" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="E6" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="G5" s="1" t="s">
+    </row>
+    <row r="7" spans="3:7" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="C7" s="1" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="6" spans="3:7" ht="25.5">
-      <c r="C6" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="E7" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="G7" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="G6" s="1" t="s">
+    </row>
+    <row r="8" spans="3:7" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="C8" s="1" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="7" spans="3:7" ht="25.5">
-      <c r="C7" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="E8" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="G8" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="G7" s="1" t="s">
+    </row>
+    <row r="9" spans="3:7" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="C9" s="1" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="8" spans="3:7" ht="25.5">
-      <c r="C8" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="E9" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="G8" s="1" t="s">
+    </row>
+    <row r="10" spans="3:7" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="C10" s="1" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="9" spans="3:7" ht="25.5">
-      <c r="C9" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="E10" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="G10" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="G9" s="1" t="s">
+    </row>
+    <row r="11" spans="3:7" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="C11" s="1" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="10" spans="3:7" ht="25.5">
-      <c r="C10" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="E11" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="G11" s="1" t="s">
         <v>174</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="11" spans="3:7" ht="25.5">
-      <c r="C11" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>178</v>
       </c>
     </row>
   </sheetData>
@@ -4537,12 +5369,12 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="C3:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="24" customWidth="1"/>
     <col min="4" max="5" width="15" customWidth="1"/>
@@ -4551,96 +5383,96 @@
     <col min="8" max="8" width="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:8">
-      <c r="C3" s="16" t="s">
+    <row r="3" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C3" s="21" t="s">
         <v>85</v>
       </c>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16" t="s">
-        <v>179</v>
-      </c>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
-    </row>
-    <row r="4" spans="3:8">
+      <c r="D3" s="21"/>
+      <c r="E3" s="21" t="s">
+        <v>175</v>
+      </c>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
+    </row>
+    <row r="4" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C4" s="13" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="F4" s="13" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="G4" s="13" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="H4" s="13" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="3:8">
+    <row r="5" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C5" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="6" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C6" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="H5" s="1" t="s">
+      <c r="F6" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="H6" s="1" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="6" spans="3:8">
-      <c r="C6" s="1" t="s">
+    <row r="7" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C7" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="H6" s="1" t="s">
+      <c r="F7" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="H7" s="1" t="s">
         <v>188</v>
-      </c>
-    </row>
-    <row r="7" spans="3:8">
-      <c r="C7" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>192</v>
       </c>
     </row>
   </sheetData>
@@ -4656,44 +5488,44 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="B2:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="150" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:2">
+    <row r="2" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B2" s="14" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2" ht="140.25" x14ac:dyDescent="0.2">
+      <c r="B3" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B4" s="14" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="B5" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B6" s="14" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="3" spans="2:2" ht="140.25">
-      <c r="B3" s="1" t="s">
+    <row r="7" spans="2:2" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="B7" s="1" t="s">
         <v>194</v>
-      </c>
-    </row>
-    <row r="4" spans="2:2">
-      <c r="B4" s="14" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="5" spans="2:2" ht="25.5">
-      <c r="B5" s="1" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="6" spans="2:2">
-      <c r="B6" s="14" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="7" spans="2:2" ht="38.25">
-      <c r="B7" s="1" t="s">
-        <v>198</v>
       </c>
     </row>
   </sheetData>
@@ -4702,15 +5534,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F494F4030F39954381FEDCB9F1521453" ma:contentTypeVersion="8" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="27a32a75921fafc58b02df1cc725ea53">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c9309f2a-e493-41e5-bc1f-ce1ae85ad224" xmlns:ns3="d8b013f3-f757-4442-942f-c178d59a4411" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8dd320713f27671350e0900a33d7d303" ns2:_="" ns3:_="">
     <xsd:import namespace="c9309f2a-e493-41e5-bc1f-ce1ae85ad224"/>
@@ -4901,6 +5724,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -4908,14 +5740,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8AE33A9A-66D9-477A-A330-1BA7B05F5338}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2E6C1B29-E2B3-4B88-B119-41B5B83630F5}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4930,6 +5754,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8AE33A9A-66D9-477A-A330-1BA7B05F5338}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>